<commit_message>
EF new plot and updated baseline support
Created an alternate EF sim file to create new plot compare options. Also adding updates to baseline support files.
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/LiteratureProjections/old_to_delete/NREL_Energy_Futures_2018.xlsx
+++ b/PV_ICE/baselines/LiteratureProjections/old_to_delete/NREL_Energy_Futures_2018.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\LiteratureProjections\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\LiteratureProjections\old_to_delete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C73CF3-6FA8-4DDF-8AAB-93E72909BA84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6299CEA-ED71-4DBE-B9BA-06D155930AD7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29940" yWindow="765" windowWidth="22575" windowHeight="11670" xr2:uid="{AF72BD23-974C-4E35-956F-C0D9DFB4E55E}"/>
+    <workbookView xWindow="29280" yWindow="-1890" windowWidth="27210" windowHeight="14085" xr2:uid="{AF72BD23-974C-4E35-956F-C0D9DFB4E55E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
   <si>
     <t>Rooftop PV_GW</t>
   </si>
@@ -52,19 +52,10 @@
     <t>Low-RE-Cost-HighElectrification</t>
   </si>
   <si>
-    <t>BaseCase_PV total_GW</t>
-  </si>
-  <si>
-    <t>Low-RE-Cost-HighElectrification_PV total_GW</t>
-  </si>
-  <si>
     <t>BaseCase_AnnualPVInstalls_GW</t>
   </si>
   <si>
     <t>Low-RE-Cost-HighElectrification_AnnualPVInstalls_GW</t>
-  </si>
-  <si>
-    <t>BaseCase_AnnualPVInstalls_MW</t>
   </si>
   <si>
     <t>Annual GW</t>
@@ -102,15 +93,30 @@
   <si>
     <t>Paper Digitized current PV ICE RUN</t>
   </si>
+  <si>
+    <t>High Electrification</t>
+  </si>
+  <si>
+    <t>tion S</t>
+  </si>
+  <si>
+    <t>IRENA 2016</t>
+  </si>
+  <si>
+    <t>IRENA 2016, global</t>
+  </si>
+  <si>
+    <t>CSA 2020</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +128,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF00BFBF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -199,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -207,20 +227,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00BFBF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -262,14 +289,17 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>BaseCase_PV total_GW</c:v>
+                  <c:v>Reference</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -508,14 +538,14 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Low-RE-Cost-HighElectrification_PV total_GW</c:v>
+                  <c:v>High Electrification</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:srgbClr val="00BFBF"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -642,11 +672,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$2</c:f>
+              <c:f>Sheet1!$S$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Current Baseline Installs GW</c:v>
+                  <c:v>CSA 2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -663,115 +693,19 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$3:$P$35</c:f>
+              <c:f>Sheet1!$S$3:$S$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
-                <c:pt idx="0">
-                  <c:v>7.7620726260000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13.385895329999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>14.903790000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16.455560000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15.227229999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15.224020000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>16.634430000000002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>18.114894270000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>19.727119859999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>21.482833530000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>23.39480571</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>25.476943420000001</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>27.74439138</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>30.213642220000001</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>32.902656369999995</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>35.830992789999996</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>39.019951150000004</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>42.4927268</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>46.274579489999994</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>50.393017059999998</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>54.877995580000004</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>59.762137190000004</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>65.080967400000006</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>70.873173500000007</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>77.180885939999996</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>84.049984789999996</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>91.530433430000002</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>99.676642009999995</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>108.5478631</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>118.208623</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>128.72919039999999</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>140.18608840000002</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>152.6626502</c:v>
+                  <c:v>437</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F19E-4AEE-A310-1F7027796D25}"/>
+              <c16:uniqueId val="{00000002-85F1-41E6-A6DB-15985A0262DD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -784,7 +718,6 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
         <c:axId val="524197968"/>
         <c:axId val="857263344"/>
       </c:barChart>
@@ -817,16 +750,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -867,21 +797,18 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Nameplate Installed Capacity [GW]</a:t>
+                  <a:t>Cumulative Installed Capacity [GW]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -899,16 +826,13 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -931,16 +855,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -960,6 +881,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12703127873347039"/>
+          <c:y val="0.16783216783216784"/>
+          <c:w val="0.24513213477070731"/>
+          <c:h val="0.34894006946392037"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -973,16 +904,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -1013,7 +941,14 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1050">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+          <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1854,8 +1789,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.8510738621901215E-3"/>
-          <c:y val="2.7906976744186046E-2"/>
+          <c:x val="2.2638900309963298E-2"/>
+          <c:y val="5.5440531706474554E-2"/>
           <c:w val="0.97393838488789852"/>
           <c:h val="0.15000109869987183"/>
         </c:manualLayout>
@@ -3016,16 +2951,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>237772</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>119945</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>22225</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>88194</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>172860</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3052,16 +2987,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>69849</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>96837</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>317147</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>181503</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>571499</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>112712</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>208139</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>13934</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3386,10 +3321,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4C04AA-A87F-4009-A208-8E065D631FDB}">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AL15" sqref="AK14:AL15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3406,7 +3342,7 @@
     <col min="14" max="14" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3420,10 +3356,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>4</v>
@@ -3435,16 +3371,19 @@
         <v>4</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3455,13 +3394,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>0</v>
@@ -3470,20 +3409,26 @@
         <v>2</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="P2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="R2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -3539,7 +3484,7 @@
         <v>7.7620726260000001</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2019</v>
       </c>
@@ -3583,7 +3528,7 @@
         <v>13.385895329999999</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -3602,7 +3547,7 @@
         <v>70941.9970623962</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" ref="F4:F34" si="7">D6-D5</f>
+        <f t="shared" ref="F5:F34" si="7">D6-D5</f>
         <v>13.624789964707148</v>
       </c>
       <c r="G5" s="3">
@@ -3638,8 +3583,11 @@
         <f t="shared" si="5"/>
         <v>14.903790000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R5">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2021</v>
       </c>
@@ -3683,7 +3631,7 @@
         <v>16.455560000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2022</v>
       </c>
@@ -3739,7 +3687,7 @@
         <v>15.227229999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2023</v>
       </c>
@@ -3783,7 +3731,7 @@
         <v>15.224020000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2024</v>
       </c>
@@ -3839,7 +3787,7 @@
         <v>16.634430000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2025</v>
       </c>
@@ -3882,8 +3830,11 @@
         <f t="shared" si="5"/>
         <v>18.114894270000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R10">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2026</v>
       </c>
@@ -3939,7 +3890,7 @@
         <v>19.727119859999998</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2027</v>
       </c>
@@ -3983,7 +3934,7 @@
         <v>21.482833530000001</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2028</v>
       </c>
@@ -4039,7 +3990,7 @@
         <v>23.39480571</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2029</v>
       </c>
@@ -4083,7 +4034,7 @@
         <v>25.476943420000001</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2030</v>
       </c>
@@ -4138,8 +4089,14 @@
         <f t="shared" si="5"/>
         <v>27.74439138</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R15">
+        <v>1632</v>
+      </c>
+      <c r="S15">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2031</v>
       </c>
@@ -4183,7 +4140,7 @@
         <v>30.213642220000001</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2032</v>
       </c>
@@ -4239,7 +4196,7 @@
         <v>32.902656369999995</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2033</v>
       </c>
@@ -4283,7 +4240,7 @@
         <v>35.830992789999996</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2034</v>
       </c>
@@ -4339,7 +4296,7 @@
         <v>39.019951150000004</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2035</v>
       </c>
@@ -4382,8 +4339,11 @@
         <f t="shared" si="5"/>
         <v>42.4927268</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R20">
+        <v>2225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2036</v>
       </c>
@@ -4439,7 +4399,7 @@
         <v>46.274579489999994</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2037</v>
       </c>
@@ -4483,7 +4443,7 @@
         <v>50.393017059999998</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2038</v>
       </c>
@@ -4539,7 +4499,7 @@
         <v>54.877995580000004</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2039</v>
       </c>
@@ -4583,7 +4543,7 @@
         <v>59.762137190000004</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2040</v>
       </c>
@@ -4638,8 +4598,11 @@
         <f t="shared" si="5"/>
         <v>65.080967400000006</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R25">
+        <v>2895</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2041</v>
       </c>
@@ -4683,7 +4646,7 @@
         <v>70.873173500000007</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2042</v>
       </c>
@@ -4739,7 +4702,7 @@
         <v>77.180885939999996</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2043</v>
       </c>
@@ -4783,7 +4746,7 @@
         <v>84.049984789999996</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2044</v>
       </c>
@@ -4839,7 +4802,7 @@
         <v>91.530433430000002</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2045</v>
       </c>
@@ -4882,8 +4845,11 @@
         <f t="shared" si="5"/>
         <v>99.676642009999995</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="R30">
+        <v>3654</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2046</v>
       </c>
@@ -4939,7 +4905,7 @@
         <v>108.5478631</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2047</v>
       </c>
@@ -4983,7 +4949,7 @@
         <v>118.208623</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2048</v>
       </c>
@@ -5039,7 +5005,7 @@
         <v>128.72919039999999</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2049</v>
       </c>
@@ -5083,7 +5049,7 @@
         <v>140.18608840000002</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2050</v>
       </c>
@@ -5121,6 +5087,18 @@
       <c r="P35">
         <f t="shared" si="5"/>
         <v>152.6626502</v>
+      </c>
+      <c r="R35">
+        <v>4512</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="18" x14ac:dyDescent="0.4">
+      <c r="I37" s="15"/>
+    </row>
+    <row r="38" spans="1:18" ht="18" x14ac:dyDescent="0.4">
+      <c r="H38" s="15"/>
+      <c r="J38" s="16" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -5154,37 +5132,37 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -5198,7 +5176,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
@@ -5207,14 +5185,14 @@
         <v>2</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -5400,7 +5378,7 @@
         <v>125409.21120000001</v>
       </c>
       <c r="L8" s="8">
-        <f t="shared" ref="L7:L36" si="2">E8-J8</f>
+        <f t="shared" ref="L8:L36" si="2">E8-J8</f>
         <v>1.8104910850524902E-6</v>
       </c>
       <c r="M8" s="9">

</xml_diff>

<commit_message>
Updating baselines, New Baselines for PVSC
Updating with new ITRPV data for baselines, and creating some hold at 2020 and upper and lower error bars on glass thickness changes. More updates to come.
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/LiteratureProjections/old_to_delete/NREL_Energy_Futures_2018.xlsx
+++ b/PV_ICE/baselines/LiteratureProjections/old_to_delete/NREL_Energy_Futures_2018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\LiteratureProjections\old_to_delete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6299CEA-ED71-4DBE-B9BA-06D155930AD7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AA80BF-EF4E-4AB8-8671-163E5D11FCBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29280" yWindow="-1890" windowWidth="27210" windowHeight="14085" xr2:uid="{AF72BD23-974C-4E35-956F-C0D9DFB4E55E}"/>
+    <workbookView minimized="1" xWindow="31020" yWindow="120" windowWidth="14400" windowHeight="7365" xr2:uid="{AF72BD23-974C-4E35-956F-C0D9DFB4E55E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
   <si>
     <t>Rooftop PV_GW</t>
   </si>
@@ -50,12 +50,6 @@
   </si>
   <si>
     <t>Low-RE-Cost-HighElectrification</t>
-  </si>
-  <si>
-    <t>BaseCase_AnnualPVInstalls_GW</t>
-  </si>
-  <si>
-    <t>Low-RE-Cost-HighElectrification_AnnualPVInstalls_GW</t>
   </si>
   <si>
     <t>Annual GW</t>
@@ -94,9 +88,6 @@
     <t>Paper Digitized current PV ICE RUN</t>
   </si>
   <si>
-    <t>High Electrification</t>
-  </si>
-  <si>
     <t>tion S</t>
   </si>
   <si>
@@ -107,6 +98,12 @@
   </si>
   <si>
     <t>CSA 2020</t>
+  </si>
+  <si>
+    <t>EF, Reference Scenario</t>
+  </si>
+  <si>
+    <t>EF, High Electrification Scenario</t>
   </si>
 </sst>
 </file>
@@ -275,7 +272,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14350013065500597"/>
+          <c:y val="3.5978733659871344E-2"/>
+          <c:w val="0.82702847744480246"/>
+          <c:h val="0.805585589225978"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -289,7 +296,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Reference</c:v>
+                  <c:v>EF, Reference Scenario</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -538,7 +545,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>High Electrification</c:v>
+                  <c:v>EF, High Electrification Scenario</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -750,7 +757,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -797,7 +804,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -826,7 +833,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -855,7 +862,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -887,7 +894,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.12703127873347039"/>
           <c:y val="0.16783216783216784"/>
-          <c:w val="0.24513213477070731"/>
+          <c:w val="0.42130608892426485"/>
           <c:h val="0.34894006946392037"/>
         </c:manualLayout>
       </c:layout>
@@ -904,7 +911,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -941,7 +948,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1050">
+        <a:defRPr sz="1200">
           <a:solidFill>
             <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
@@ -977,7 +984,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1040541553609205"/>
+          <c:y val="4.1698054148709703E-2"/>
+          <c:w val="0.86617410177095544"/>
+          <c:h val="0.78959023509961757"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -991,14 +1008,17 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>BaseCase_AnnualPVInstalls_GW</c:v>
+                  <c:v>EF, Reference Scenario</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1008,10 +1028,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$34</c:f>
+              <c:f>Sheet1!$A$3:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>2018</c:v>
                 </c:pt>
@@ -1107,16 +1127,19 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2050</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$34</c:f>
+              <c:f>Sheet1!$F$3:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>6.8032972931708002</c:v>
                 </c:pt>
@@ -1231,14 +1254,14 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Low-RE-Cost-HighElectrification_AnnualPVInstalls_GW</c:v>
+                  <c:v>EF, High Electrification Scenario</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:srgbClr val="00BFBF"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1248,10 +1271,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$34</c:f>
+              <c:f>Sheet1!$A$3:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>2018</c:v>
                 </c:pt>
@@ -1347,16 +1370,19 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2050</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$3:$L$34</c:f>
+              <c:f>Sheet1!$L$3:$L$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>14.861307561989449</c:v>
                 </c:pt>
@@ -1459,144 +1485,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-605B-4F88-800A-F58DB6841749}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$P$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Current Baseline Installs GW</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$P$3:$P$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="33"/>
-                <c:pt idx="0">
-                  <c:v>7.7620726260000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13.385895329999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>14.903790000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16.455560000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15.227229999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15.224020000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>16.634430000000002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>18.114894270000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>19.727119859999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>21.482833530000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>23.39480571</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>25.476943420000001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>27.74439138</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>30.213642220000001</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>32.902656369999995</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>35.830992789999996</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>39.019951150000004</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>42.4927268</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>46.274579489999994</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>50.393017059999998</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>54.877995580000004</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>59.762137190000004</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>65.080967400000006</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>70.873173500000007</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>77.180885939999996</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>84.049984789999996</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>91.530433430000002</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>99.676642009999995</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>108.5478631</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>118.208623</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>128.72919039999999</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>140.18608840000002</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>152.6626502</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-409D-47DB-BC7A-0352D5C1EE6E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1609,7 +1497,6 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
         <c:axId val="518702640"/>
         <c:axId val="518704608"/>
       </c:barChart>
@@ -1642,16 +1529,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1692,16 +1576,13 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
@@ -1724,16 +1605,13 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -1756,16 +1634,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1789,10 +1664,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.2638900309963298E-2"/>
-          <c:y val="5.5440531706474554E-2"/>
-          <c:w val="0.97393838488789852"/>
-          <c:h val="0.15000109869987183"/>
+          <c:x val="0.46972063374390027"/>
+          <c:y val="6.3925569325775172E-2"/>
+          <c:w val="0.49994536151177466"/>
+          <c:h val="0.18818392001060966"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1808,16 +1683,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -1848,7 +1720,14 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1200">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+          <a:ea typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="DejaVu Sans Condensed" panose="020B0606030804020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -2952,15 +2831,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>237772</xdr:colOff>
+      <xdr:colOff>240948</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>119945</xdr:rowOff>
+      <xdr:rowOff>123119</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>88194</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>172860</xdr:rowOff>
+      <xdr:colOff>87842</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>148167</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2987,16 +2866,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>317147</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>181503</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>635705</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>122235</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>208139</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>13934</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>137582</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3324,8 +3203,8 @@
   <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AL15" sqref="AK14:AL15"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AC38" sqref="AC38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3356,10 +3235,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>4</v>
@@ -3371,16 +3250,16 @@
         <v>4</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" t="s">
-        <v>9</v>
-      </c>
       <c r="R1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
@@ -3394,13 +3273,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>0</v>
@@ -3409,23 +3288,23 @@
         <v>2</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="O2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="S2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
@@ -5098,7 +4977,7 @@
     <row r="38" spans="1:18" ht="18" x14ac:dyDescent="0.4">
       <c r="H38" s="15"/>
       <c r="J38" s="16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -5132,37 +5011,37 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -5176,7 +5055,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
@@ -5185,14 +5064,14 @@
         <v>2</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">

</xml_diff>